<commit_message>
commiting POM framework for selenium
</commit_message>
<xml_diff>
--- a/src/main/java/com/amz/qa/testdata/TestData.xlsx
+++ b/src/main/java/com/amz/qa/testdata/TestData.xlsx
@@ -3,19 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjaiswar\Desktop\driver\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4589119F-1F33-4AF2-8FF3-E5A414307B39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{E68D9BDE-93E8-41F6-BE02-C8F4F4A14DF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{3B383FEC-6D51-44BB-ADC4-AEDD03585184}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="20670" windowHeight="11820" xr2:uid="{3B383FEC-6D51-44BB-ADC4-AEDD03585184}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTestData" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:N13"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="3">
   <si>
     <t>Username</t>
   </si>
@@ -413,10 +410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7747527F-182C-461D-AB65-A2F86E856F52}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,11 +438,104 @@
         <v>2</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>9594748758</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>9594748758</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>9594748758</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>9594748758</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>9594748758</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>9594748758</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>9594748758</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9594748758</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9594748758</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{9B1D9467-5F47-418C-86F0-C9EBB7812B06}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{E73A73BA-8DD6-4A16-8B23-2065622FD840}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{07F32638-A514-4C24-8055-733E8661BE52}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{61866F99-D0B3-4A3C-A604-62EE1A993B39}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{BC984C20-8C8D-41DF-B056-3C59753AFB6F}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{EBCB91EB-8EB6-42E9-9C1D-EC3A0ED6FEFF}"/>
+    <hyperlink ref="B8" r:id="rId7" xr:uid="{783F77F1-9BF3-4EC8-AC4F-EC8A2A2D80C2}"/>
+    <hyperlink ref="B9" r:id="rId8" xr:uid="{C809295C-5BA2-4F20-9608-BAEE75D7F6E8}"/>
+    <hyperlink ref="B10" r:id="rId9" xr:uid="{712302F0-9249-46A1-9A93-AF041B741C7A}"/>
+    <hyperlink ref="B11" r:id="rId10" xr:uid="{C919248F-4DC4-4EF4-9B5C-7DF88565BB7C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0A0D395-41CC-44C2-A689-CC9DA6274876}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>